<commit_message>
Change training data from (-1, 1) to (0, 1)
</commit_message>
<xml_diff>
--- a/single_layer/training_data.xlsx
+++ b/single_layer/training_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KYLA\Documents\Projects\ANN\single_layer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC77D99C-36CC-44D1-9536-9F8BF5A095CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5179F1-C5C1-41C4-A0D5-EF35CD1C1A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F142798B-45F7-4635-B028-452368135F48}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,10 +437,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -462,7 +462,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>